<commit_message>
Planning + structure fixes
- plan improvement implementations
- fix some structuring of the Contribution part
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Segmentation of point clouds</t>
   </si>
   <si>
-    <t>Coloring of points</t>
-  </si>
-  <si>
     <t>Writing</t>
   </si>
   <si>
@@ -297,33 +294,18 @@
     <t>TESTING --&gt; what does work, what does not work</t>
   </si>
   <si>
-    <t>Explain: what does work? What does not?</t>
-  </si>
-  <si>
     <t>Implementation 2D (articulated object)</t>
   </si>
   <si>
     <t>Augmented Reality</t>
   </si>
   <si>
-    <t>Add Programming examples</t>
-  </si>
-  <si>
     <t>Find test data</t>
   </si>
   <si>
-    <t>Implement improvements</t>
-  </si>
-  <si>
     <t>Plan further improvements</t>
   </si>
   <si>
-    <t>Start with 3D functionality</t>
-  </si>
-  <si>
-    <t>Reread document!</t>
-  </si>
-  <si>
     <t>Notations, merge algorithmus</t>
   </si>
   <si>
@@ -336,10 +318,58 @@
     <t>Test positioning, selection of Atoms</t>
   </si>
   <si>
-    <t>Design</t>
-  </si>
-  <si>
     <t>Improve</t>
+  </si>
+  <si>
+    <t>UI Design</t>
+  </si>
+  <si>
+    <t>Elements: lock rotation + enlarge collider bottom</t>
+  </si>
+  <si>
+    <t>AR learning</t>
+  </si>
+  <si>
+    <t>AR learning + bug fixes</t>
+  </si>
+  <si>
+    <t>AR documentation</t>
+  </si>
+  <si>
+    <t>AR poject - functionality</t>
+  </si>
+  <si>
+    <t>AR documentation + bug fixes</t>
+  </si>
+  <si>
+    <t>points in hours</t>
+  </si>
+  <si>
+    <t>8 points per day</t>
+  </si>
+  <si>
+    <t>Coloring/Storing of points</t>
+  </si>
+  <si>
+    <t>Rewrite: what does work? What does not?</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Implement region growing + error handling</t>
+  </si>
+  <si>
+    <t>Add Programming examples + Text</t>
   </si>
 </sst>
 </file>
@@ -352,7 +382,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -426,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +559,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2FFF0C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2DF50D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -610,7 +652,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -650,8 +692,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -670,7 +716,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -694,8 +739,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -715,6 +762,8 @@
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -734,6 +783,8 @@
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1063,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N115"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1499,7 +1550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:11">
       <c r="A49" s="2">
         <v>43163</v>
       </c>
@@ -1507,7 +1558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:11">
       <c r="A50" s="2">
         <v>43164</v>
       </c>
@@ -1518,7 +1569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:11">
       <c r="A51" s="2">
         <v>43165</v>
       </c>
@@ -1529,7 +1580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:11">
       <c r="A52" s="2">
         <v>43166</v>
       </c>
@@ -1540,7 +1591,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:11">
       <c r="A53" s="2">
         <v>43167</v>
       </c>
@@ -1551,7 +1602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:11">
       <c r="A54" s="2">
         <v>43168</v>
       </c>
@@ -1559,7 +1610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:11">
       <c r="A55" s="2">
         <v>43169</v>
       </c>
@@ -1567,15 +1618,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:11">
       <c r="A56" s="2">
         <v>43170</v>
       </c>
       <c r="B56" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="2">
         <v>43171</v>
       </c>
@@ -1586,446 +1640,567 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:11">
       <c r="A58" s="2">
         <v>43172</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="23">
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58">
+        <v>8</v>
+      </c>
+      <c r="J58">
+        <v>13</v>
+      </c>
+      <c r="K58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="F60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="23">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20">
+    <row r="63" spans="1:11" ht="20">
       <c r="A63" s="2">
         <v>43179</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" thickBot="1">
+        <v>67</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="16" thickBot="1">
       <c r="A64" s="2">
         <v>43182</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="18">
       <c r="A65" s="2">
         <v>43185</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="20"/>
-      <c r="M65" s="21"/>
-    </row>
-    <row r="66" spans="1:14" ht="19" thickBot="1">
+        <v>58</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="20"/>
+    </row>
+    <row r="66" spans="1:16" ht="19" thickBot="1">
       <c r="A66" s="2">
         <v>43186</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E66" s="15"/>
-      <c r="F66" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="24"/>
+      <c r="F66" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="22"/>
+      <c r="M66" s="23"/>
       <c r="N66" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="F67" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-    </row>
-    <row r="68" spans="1:14">
+        <v>66</v>
+      </c>
+      <c r="P66">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="F67" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="2">
         <v>43192</v>
       </c>
       <c r="B68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F68" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="2">
         <v>43194</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
-      </c>
-      <c r="F69" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F69" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="2">
         <v>43195</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F70" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:16">
       <c r="A71" s="2">
         <v>43196</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F71" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
-      <c r="A72" s="39">
+    <row r="72" spans="1:16">
+      <c r="A72" s="38">
         <v>43197</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
-      <c r="A73" s="39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73" s="38">
         <v>43198</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="2">
         <v>43199</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="18">
       <c r="A75" s="2">
         <v>43200</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>66</v>
+        <v>95</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="K75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="2">
         <v>43201</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="K76">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="2">
         <v>43202</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="K77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="2">
         <v>43203</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
-      <c r="A79" s="39">
+        <v>90</v>
+      </c>
+      <c r="K78">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
+      <c r="A79" s="38">
         <v>43204</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
-      <c r="A80" s="39">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="A80" s="38">
         <v>43205</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="18">
+      <c r="B80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="18">
       <c r="A81" s="2">
         <v>43206</v>
       </c>
+      <c r="B81" t="s">
+        <v>106</v>
+      </c>
       <c r="E81" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:11">
       <c r="A82" s="2">
         <v>43207</v>
       </c>
-      <c r="F82" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="B82" t="s">
+        <v>104</v>
+      </c>
+      <c r="F82" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="2">
         <v>43208</v>
       </c>
+      <c r="B83" t="s">
+        <v>104</v>
+      </c>
       <c r="F83" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>77</v>
+      </c>
+      <c r="K83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="2">
         <v>43209</v>
       </c>
+      <c r="B84" t="s">
+        <v>103</v>
+      </c>
       <c r="F84" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>76</v>
+      </c>
+      <c r="K84">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="2">
         <v>43210</v>
       </c>
+      <c r="B85" t="s">
+        <v>102</v>
+      </c>
       <c r="F85" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="39">
+      <c r="K85">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="38">
         <v>43211</v>
       </c>
+      <c r="B86" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="F86" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="39">
+        <v>109</v>
+      </c>
+      <c r="K86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="38">
         <v>43212</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:11">
       <c r="A88" s="2">
         <v>43213</v>
       </c>
-      <c r="D88" s="35"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
-      <c r="I88" s="36"/>
-      <c r="J88" s="34"/>
-    </row>
-    <row r="89" spans="1:10" ht="18">
+      <c r="D88" s="34"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="35"/>
+      <c r="H88" s="35"/>
+      <c r="I88" s="35"/>
+      <c r="J88" s="33"/>
+    </row>
+    <row r="89" spans="1:11" ht="18">
       <c r="A89" s="2">
         <v>43214</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F89" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="F90" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="F91" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G89" s="25"/>
-      <c r="H89" s="25"/>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="F90" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="G90" s="29"/>
-      <c r="H90" s="29"/>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="F91" s="25" t="s">
+      <c r="G91" s="24"/>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="F92" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G91" s="25"/>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="F92" s="25" t="s">
+      <c r="G92" s="24"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="F93" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="G93" s="39"/>
+      <c r="H93" s="39"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="F94" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G94" s="39"/>
+      <c r="H94" s="39"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="F95" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="G92" s="25"/>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="F93" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="F94" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
-      <c r="F95" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G95" s="29"/>
-      <c r="H95" s="29"/>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="F96" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="4:7" ht="20">
-      <c r="E98" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="100" spans="4:7">
-      <c r="D100" s="33">
+      <c r="G95" s="28"/>
+      <c r="H95" s="28"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="F96" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="G96" s="40"/>
+      <c r="H96" s="40"/>
+      <c r="I96" s="40"/>
+    </row>
+    <row r="97" spans="4:9">
+      <c r="F97" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="G97" s="40"/>
+      <c r="H97" s="40"/>
+      <c r="I97" s="40"/>
+    </row>
+    <row r="98" spans="4:9" ht="20">
+      <c r="E98" s="36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9">
+      <c r="D100" s="32">
         <v>43193</v>
       </c>
-      <c r="E100" s="29" t="s">
+      <c r="E100" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+    </row>
+    <row r="101" spans="4:9">
+      <c r="E101" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+    </row>
+    <row r="102" spans="4:9">
+      <c r="E102" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
+    </row>
+    <row r="103" spans="4:9">
+      <c r="E103" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+    </row>
+    <row r="104" spans="4:9">
+      <c r="E104" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F100" s="29"/>
-      <c r="G100" s="29"/>
-    </row>
-    <row r="101" spans="4:7">
-      <c r="E101" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="F101" s="30"/>
-      <c r="G101" s="30"/>
-    </row>
-    <row r="102" spans="4:7">
-      <c r="E102" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-    </row>
-    <row r="103" spans="4:7">
-      <c r="E103" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="F103" s="38"/>
-      <c r="G103" s="38"/>
-    </row>
-    <row r="104" spans="4:7">
-      <c r="E104" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-    </row>
-    <row r="105" spans="4:7">
-      <c r="E105" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="F105" s="30"/>
-      <c r="G105" s="30"/>
-    </row>
-    <row r="106" spans="4:7">
-      <c r="E106" s="31" t="s">
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+    </row>
+    <row r="105" spans="4:9">
+      <c r="E105" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+    </row>
+    <row r="106" spans="4:9">
+      <c r="E106" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F106" s="30"/>
+      <c r="G106" s="30"/>
+    </row>
+    <row r="107" spans="4:9">
+      <c r="E107" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F106" s="31"/>
-      <c r="G106" s="31"/>
-    </row>
-    <row r="107" spans="4:7">
-      <c r="E107" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F107" s="38"/>
-      <c r="G107" s="38"/>
-    </row>
-    <row r="108" spans="4:7">
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+    </row>
+    <row r="108" spans="4:9">
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="4:7">
-      <c r="D109" s="33">
+    <row r="109" spans="4:9">
+      <c r="D109" s="32">
         <v>43200</v>
       </c>
       <c r="E109" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="110" spans="4:7">
+        <v>116</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="4:9">
       <c r="E110" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="111" spans="4:7">
+        <v>110</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="4:9">
       <c r="E111" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="112" spans="4:7">
+        <v>115</v>
+      </c>
+      <c r="F111">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="4:9">
       <c r="E112" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="113" spans="5:5">
+        <v>93</v>
+      </c>
+      <c r="F112">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="5:11">
       <c r="E113" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="114" spans="5:5">
-      <c r="E114" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="115" spans="5:5">
-      <c r="E115" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="F113">
+        <v>5</v>
+      </c>
+      <c r="H113" t="s">
+        <v>111</v>
+      </c>
+      <c r="I113" t="s">
+        <v>112</v>
+      </c>
+      <c r="J113" t="s">
+        <v>113</v>
+      </c>
+      <c r="K113" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="114" spans="5:11">
+      <c r="F114" s="8">
+        <f>SUM(F109:F113)</f>
+        <v>29</v>
+      </c>
+      <c r="H114">
+        <v>3</v>
+      </c>
+      <c r="I114">
+        <v>3</v>
+      </c>
+      <c r="J114">
+        <v>5</v>
+      </c>
+      <c r="K114">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create classes for LRP
- package LRP
- ToDo: Plan algorithm
- Rewrite ICP, ClusterTree, ...
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:CRTarget Flags="8192"/>
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -408,29 +409,37 @@
     <t>Implement Region growing from LRP</t>
   </si>
   <si>
-    <t>Find/Write paper Sensors</t>
-  </si>
-  <si>
-    <t>Find/Write papers non-rigid registration</t>
-  </si>
-  <si>
-    <t>Write Scanning, Reconstruction + Paper general</t>
-  </si>
-  <si>
-    <t>Find/Write papers Shape fitting/Elipsoid fitting</t>
+    <t>Collect all State of the Art papers</t>
+  </si>
+  <si>
+    <t>Collect Non-rigid registration papers</t>
+  </si>
+  <si>
+    <t>Write Non-rigid registration papers</t>
+  </si>
+  <si>
+    <t>Implement elipse fitting</t>
+  </si>
+  <si>
+    <t>Write State of the Art + Structure</t>
+  </si>
+  <si>
+    <t>Create test data</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -503,8 +512,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +653,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF22FF10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2CFF0F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -718,7 +746,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,8 +798,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -820,8 +852,11 @@
     <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -847,6 +882,8 @@
     <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -872,6 +909,8 @@
     <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1204,7 +1243,7 @@
   <dimension ref="A1:P135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2308,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="4:10">
+    <row r="113" spans="2:10">
       <c r="E113" s="42" t="s">
         <v>94</v>
       </c>
@@ -2316,7 +2355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="4:10">
+    <row r="114" spans="2:10">
       <c r="E114" s="41" t="s">
         <v>113</v>
       </c>
@@ -2324,13 +2363,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="4:10">
+    <row r="115" spans="2:10">
       <c r="F115" s="8">
         <f>SUM(F109:F114)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="4:10">
+    <row r="117" spans="2:10">
       <c r="D117" s="32">
         <v>43214</v>
       </c>
@@ -2345,7 +2384,7 @@
       </c>
       <c r="J117" s="44"/>
     </row>
-    <row r="118" spans="4:10">
+    <row r="118" spans="2:10">
       <c r="E118" t="s">
         <v>115</v>
       </c>
@@ -2353,7 +2392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="4:10">
+    <row r="119" spans="2:10">
       <c r="E119" t="s">
         <v>128</v>
       </c>
@@ -2361,7 +2400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="4:10">
+    <row r="120" spans="2:10">
       <c r="E120" t="s">
         <v>116</v>
       </c>
@@ -2375,7 +2414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="4:10">
+    <row r="121" spans="2:10">
       <c r="E121" t="s">
         <v>61</v>
       </c>
@@ -2385,8 +2424,11 @@
       <c r="I121" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="122" spans="4:10">
+      <c r="J121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:10">
       <c r="E122" t="s">
         <v>117</v>
       </c>
@@ -2396,43 +2438,52 @@
       <c r="I122" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="123" spans="4:10">
-      <c r="E123" t="s">
-        <v>131</v>
-      </c>
-      <c r="F123">
-        <v>4</v>
+      <c r="J122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:10">
+      <c r="E123" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="F123" s="46">
+        <v>2</v>
       </c>
       <c r="I123" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="124" spans="4:10">
+      <c r="J123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="B124" t="s">
+        <v>135</v>
+      </c>
       <c r="E124" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F124">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I124" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="4:10">
-      <c r="E125" t="s">
-        <v>132</v>
-      </c>
-      <c r="F125">
+    <row r="125" spans="2:10">
+      <c r="E125" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F125" s="48">
         <v>2</v>
       </c>
       <c r="I125" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="4:10">
+    <row r="126" spans="2:10">
       <c r="E126" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F126">
         <v>4</v>
@@ -2441,52 +2492,70 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" spans="4:10">
+    <row r="127" spans="2:10">
+      <c r="D127" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E127" t="s">
+        <v>132</v>
+      </c>
+      <c r="F127">
+        <v>8</v>
+      </c>
       <c r="J127" s="8">
         <f xml:space="preserve"> SUM(J120:J126)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="128" spans="4:10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="2:10">
+      <c r="D128" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E128" t="s">
+        <v>134</v>
+      </c>
       <c r="F128">
-        <f>SUM(F117:F126)</f>
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I128" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="9:10">
+    <row r="129" spans="6:10">
+      <c r="F129">
+        <f>SUM(F117:F128)</f>
+        <v>54</v>
+      </c>
       <c r="I129" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="9:10">
+    <row r="130" spans="6:10">
       <c r="I130" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="9:10">
+    <row r="131" spans="6:10">
       <c r="I131" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="9:10">
+    <row r="132" spans="6:10">
       <c r="I132" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="9:10">
+    <row r="133" spans="6:10">
       <c r="I133" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="9:10">
+    <row r="134" spans="6:10">
       <c r="I134" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="9:10">
+    <row r="135" spans="6:10">
       <c r="J135" s="8">
         <f xml:space="preserve"> SUM(J128:J134)</f>
         <v>0</v>
@@ -2494,22 +2563,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J127">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="10"/>
+        <cfvo type="num" val="20"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="10"/>
-        <cfvo type="num" val="20"/>
-        <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>

</xml_diff>

<commit_message>
Implement ICP + LRP
- first version!!
- ToDo: Ransac + region growing
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>Write LRP algorithm</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1242,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="F133" sqref="F133"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="K130" sqref="K130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2387,10 +2389,10 @@
       <c r="J117" s="44"/>
     </row>
     <row r="118" spans="2:10">
-      <c r="E118" t="s">
+      <c r="E118" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="F118">
+      <c r="F118" s="45">
         <v>6</v>
       </c>
     </row>
@@ -2403,168 +2405,179 @@
       </c>
     </row>
     <row r="120" spans="2:10">
-      <c r="E120" t="s">
-        <v>116</v>
-      </c>
-      <c r="F120">
-        <v>4</v>
-      </c>
-      <c r="I120" t="s">
-        <v>121</v>
-      </c>
-      <c r="J120">
-        <v>5</v>
+      <c r="E120" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="F120" s="49">
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="2:10">
       <c r="E121" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="F121">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J121">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="2:10">
       <c r="E122" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="F122">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I122" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J122">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="2:10">
-      <c r="E123" s="46" t="s">
+      <c r="E123" t="s">
+        <v>117</v>
+      </c>
+      <c r="F123">
+        <v>4</v>
+      </c>
+      <c r="I123" t="s">
+        <v>123</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="E124" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="F123" s="46">
+      <c r="F124" s="46">
         <v>2</v>
       </c>
-      <c r="I123" t="s">
+      <c r="I124" t="s">
         <v>124</v>
       </c>
-      <c r="J123">
+      <c r="J124">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="2:10">
-      <c r="B124" t="s">
+    <row r="125" spans="2:10">
+      <c r="B125" t="s">
         <v>135</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E125" t="s">
         <v>133</v>
       </c>
-      <c r="F124">
+      <c r="F125">
         <v>6</v>
       </c>
-      <c r="I124" t="s">
+      <c r="I125" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="125" spans="2:10">
-      <c r="E125" s="48" t="s">
+      <c r="J125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10">
+      <c r="E126" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="F125" s="48">
+      <c r="F126" s="48">
         <v>2</v>
       </c>
-      <c r="I125" t="s">
+      <c r="I126" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="2:10">
-      <c r="E126" t="s">
+    <row r="127" spans="2:10">
+      <c r="E127" t="s">
         <v>131</v>
       </c>
-      <c r="F126">
+      <c r="F127">
         <v>4</v>
       </c>
-      <c r="I126" t="s">
+      <c r="I127" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="127" spans="2:10">
-      <c r="D127" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="E127" t="s">
-        <v>132</v>
-      </c>
-      <c r="F127">
-        <v>8</v>
-      </c>
-      <c r="J127" s="8">
-        <f xml:space="preserve"> SUM(J120:J126)</f>
-        <v>10</v>
       </c>
     </row>
     <row r="128" spans="2:10">
       <c r="D128" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="E128" s="49" t="s">
+      <c r="E128" t="s">
+        <v>132</v>
+      </c>
+      <c r="F128">
+        <v>8</v>
+      </c>
+      <c r="J128" s="8">
+        <f xml:space="preserve"> SUM(J121:J127)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="4:10">
+      <c r="D129" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E129" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="F128" s="49">
+      <c r="F129" s="49">
         <v>3</v>
       </c>
-      <c r="I128" t="s">
+      <c r="I129" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="6:10">
-      <c r="F129">
-        <f>SUM(F117:F128)</f>
-        <v>54</v>
-      </c>
-      <c r="I129" t="s">
+    <row r="130" spans="4:10">
+      <c r="F130">
+        <f>SUM(F117:F129)</f>
+        <v>60</v>
+      </c>
+      <c r="I130" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="6:10">
-      <c r="I130" t="s">
+    <row r="131" spans="4:10">
+      <c r="I131" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="6:10">
-      <c r="I131" t="s">
+    <row r="132" spans="4:10">
+      <c r="I132" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="6:10">
-      <c r="I132" t="s">
+    <row r="133" spans="4:10">
+      <c r="I133" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="6:10">
-      <c r="I133" t="s">
+    <row r="134" spans="4:10">
+      <c r="I134" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="6:10">
-      <c r="I134" t="s">
+    <row r="135" spans="4:10">
+      <c r="I135" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="6:10">
-      <c r="J135" s="8">
-        <f xml:space="preserve"> SUM(J128:J134)</f>
+    <row r="136" spans="4:10">
+      <c r="J136" s="8">
+        <f xml:space="preserve"> SUM(J129:J135)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J127">
+  <conditionalFormatting sqref="J128">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2586,7 +2599,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J135">
+  <conditionalFormatting sqref="J136">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Structure thesis + Normal estimation
- write about normal estimation
- implement first draft (excluding solver)
- write TODOs for thesis + structure chapters
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="146">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>Create images "Introduction"</t>
+  </si>
+  <si>
+    <t>halfed</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C115" workbookViewId="0">
-      <selection activeCell="E140" sqref="E140"/>
+    <sheetView tabSelected="1" topLeftCell="B113" workbookViewId="0">
+      <selection activeCell="K145" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2604,7 +2607,10 @@
         <v>136</v>
       </c>
       <c r="F129" s="51">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G129" t="s">
+        <v>145</v>
       </c>
       <c r="I129" t="s">
         <v>120</v>
@@ -2614,11 +2620,14 @@
       </c>
     </row>
     <row r="130" spans="4:10">
-      <c r="E130" t="s">
+      <c r="E130" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="F130">
-        <v>4</v>
+      <c r="F130" s="51">
+        <v>2</v>
+      </c>
+      <c r="G130" t="s">
+        <v>145</v>
       </c>
       <c r="I130" t="s">
         <v>121</v>
@@ -2720,36 +2729,54 @@
     <row r="138" spans="4:10">
       <c r="F138">
         <f>SUM(F129:F137)</f>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I138" t="s">
         <v>120</v>
+      </c>
+      <c r="J138" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="4:10">
       <c r="I139" t="s">
         <v>121</v>
       </c>
+      <c r="J139" s="14" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="140" spans="4:10">
       <c r="I140" t="s">
         <v>122</v>
       </c>
+      <c r="J140" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="141" spans="4:10">
       <c r="I141" t="s">
         <v>123</v>
       </c>
+      <c r="J141" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="142" spans="4:10">
       <c r="I142" t="s">
         <v>124</v>
       </c>
+      <c r="J142" s="14" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="143" spans="4:10">
       <c r="I143" t="s">
         <v>125</v>
       </c>
+      <c r="J143" s="14" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="144" spans="4:10">
       <c r="I144" t="s">
@@ -2759,7 +2786,7 @@
     <row r="145" spans="9:10">
       <c r="J145" s="8">
         <f xml:space="preserve"> SUM(J138:J144)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="9:10">

</xml_diff>

<commit_message>
Summarize State of the Art
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="158">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -478,9 +478,6 @@
     <t>Include head to pose</t>
   </si>
   <si>
-    <t>Fix RANSAC --&gt; same number of points!</t>
-  </si>
-  <si>
     <t>Check histogram formular (FPFH)</t>
   </si>
   <si>
@@ -491,6 +488,12 @@
   </si>
   <si>
     <t>First thesis version + correction</t>
+  </si>
+  <si>
+    <t>Create new dataset --&gt; more points, different shapes?</t>
+  </si>
+  <si>
+    <t>Write State of the Art</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -834,8 +836,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -981,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1025,6 +1029,7 @@
     <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1068,6 +1073,7 @@
     <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1397,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P173"/>
+  <dimension ref="A1:P184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2862,156 +2868,152 @@
     </row>
     <row r="142" spans="4:10">
       <c r="E142" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="F142">
-        <v>4</v>
-      </c>
-      <c r="I142" t="s">
-        <v>124</v>
-      </c>
-      <c r="J142" s="14" t="s">
-        <v>86</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J142" s="14"/>
     </row>
     <row r="143" spans="4:10">
       <c r="E143" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F143">
         <v>4</v>
       </c>
       <c r="I143" t="s">
-        <v>125</v>
-      </c>
-      <c r="J143" s="14">
-        <v>4</v>
+        <v>124</v>
+      </c>
+      <c r="J143" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="144" spans="4:10">
       <c r="E144" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F144">
         <v>4</v>
       </c>
-      <c r="J144" s="14"/>
+      <c r="I144" t="s">
+        <v>125</v>
+      </c>
+      <c r="J144" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="145" spans="4:10">
-      <c r="E145" s="51" t="s">
+      <c r="E145" t="s">
+        <v>153</v>
+      </c>
+      <c r="F145">
+        <v>4</v>
+      </c>
+      <c r="J145" s="14"/>
+    </row>
+    <row r="146" spans="4:10">
+      <c r="E146" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="F145" s="51">
+      <c r="F146" s="51">
         <v>4</v>
       </c>
-      <c r="J145" s="14"/>
-    </row>
-    <row r="146" spans="4:10">
-      <c r="E146" t="s">
+      <c r="J146" s="14"/>
+    </row>
+    <row r="147" spans="4:10">
+      <c r="E147" t="s">
         <v>149</v>
       </c>
-      <c r="F146">
+      <c r="F147">
         <v>6</v>
       </c>
-      <c r="I146" t="s">
+      <c r="I147" t="s">
         <v>126</v>
       </c>
-      <c r="J146" s="14">
+      <c r="J147" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="4:10">
-      <c r="F147">
-        <f>SUM(F140:F146)</f>
-        <v>38</v>
-      </c>
-      <c r="J147" s="8">
-        <f xml:space="preserve"> SUM(J138:J146)</f>
+    <row r="148" spans="4:10">
+      <c r="F148">
+        <f>SUM(F140:F147)</f>
+        <v>46</v>
+      </c>
+      <c r="J148" s="8">
+        <f xml:space="preserve"> SUM(J138:J147)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="4:10">
-      <c r="I148" t="s">
+    <row r="149" spans="4:10">
+      <c r="I149" t="s">
         <v>120</v>
       </c>
-      <c r="J148" s="14">
+      <c r="J149" s="14">
         <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="4:10">
-      <c r="D149" s="32">
-        <v>43252</v>
-      </c>
-      <c r="E149" t="s">
-        <v>155</v>
-      </c>
-      <c r="F149">
-        <v>3</v>
-      </c>
-      <c r="I149" t="s">
-        <v>121</v>
-      </c>
-      <c r="J149" s="14">
-        <v>3</v>
       </c>
     </row>
     <row r="150" spans="4:10">
       <c r="D150" s="32">
+        <v>43252</v>
+      </c>
+      <c r="E150" t="s">
+        <v>154</v>
+      </c>
+      <c r="F150">
+        <v>3</v>
+      </c>
+      <c r="I150" t="s">
+        <v>121</v>
+      </c>
+      <c r="J150" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="4:10">
+      <c r="D151" s="32">
         <v>43255</v>
       </c>
-      <c r="E150" t="s">
-        <v>156</v>
-      </c>
-      <c r="F150">
+      <c r="E151" t="s">
+        <v>155</v>
+      </c>
+      <c r="F151">
         <v>5</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I151" t="s">
         <v>122</v>
       </c>
-      <c r="J150" s="14">
+      <c r="J151" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="4:10">
-      <c r="E151" s="48"/>
-      <c r="I151" t="s">
+    <row r="152" spans="4:10">
+      <c r="E152" s="48"/>
+      <c r="I152" t="s">
         <v>123</v>
       </c>
-      <c r="J151" s="14">
+      <c r="J152" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="4:10">
-      <c r="D152" s="26" t="s">
+    <row r="153" spans="4:10">
+      <c r="D153" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E152" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="I152" t="s">
+      <c r="E153" s="48"/>
+      <c r="I153" t="s">
         <v>124</v>
       </c>
-      <c r="J152">
+      <c r="J153">
         <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="4:10">
-      <c r="E153" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="I153" t="s">
-        <v>125</v>
-      </c>
-      <c r="J153">
-        <v>3</v>
       </c>
     </row>
     <row r="154" spans="4:10">
       <c r="E154" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I154" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J154">
         <v>3</v>
@@ -3019,32 +3021,40 @@
     </row>
     <row r="155" spans="4:10">
       <c r="E155" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="J155" s="8">
-        <f xml:space="preserve"> SUM(J148:J154)</f>
+        <v>151</v>
+      </c>
+      <c r="I155" t="s">
+        <v>126</v>
+      </c>
+      <c r="J155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="4:10">
+      <c r="E156" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="J156" s="8">
+        <f xml:space="preserve"> SUM(J149:J155)</f>
         <v>20</v>
       </c>
     </row>
     <row r="157" spans="4:10">
-      <c r="I157" t="s">
-        <v>120</v>
-      </c>
-      <c r="J157" s="14">
-        <v>4</v>
+      <c r="E157" s="48" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="4:10">
       <c r="I158" t="s">
-        <v>121</v>
-      </c>
-      <c r="J158" s="14" t="s">
-        <v>86</v>
+        <v>120</v>
+      </c>
+      <c r="J158" s="14">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="4:10">
       <c r="I159" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J159" s="14" t="s">
         <v>86</v>
@@ -3052,7 +3062,7 @@
     </row>
     <row r="160" spans="4:10">
       <c r="I160" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J160" s="14" t="s">
         <v>86</v>
@@ -3060,83 +3070,164 @@
     </row>
     <row r="161" spans="9:10">
       <c r="I161" t="s">
-        <v>124</v>
-      </c>
-      <c r="J161">
-        <v>3</v>
+        <v>123</v>
+      </c>
+      <c r="J161" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="162" spans="9:10">
       <c r="I162" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J162">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="9:10">
       <c r="I163" t="s">
+        <v>125</v>
+      </c>
+      <c r="J163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="9:10">
+      <c r="I164" t="s">
         <v>126</v>
       </c>
-      <c r="J163">
+      <c r="J164">
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="9:10">
-      <c r="J164" s="8">
-        <f xml:space="preserve"> SUM(J157:J163)</f>
+    <row r="165" spans="9:10">
+      <c r="J165" s="8">
+        <f xml:space="preserve"> SUM(J158:J164)</f>
         <v>10</v>
-      </c>
-    </row>
-    <row r="166" spans="9:10">
-      <c r="I166" t="s">
-        <v>120</v>
-      </c>
-      <c r="J166" s="14">
-        <v>2</v>
       </c>
     </row>
     <row r="167" spans="9:10">
       <c r="I167" t="s">
-        <v>121</v>
-      </c>
-      <c r="J167" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="J167" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="168" spans="9:10">
       <c r="I168" t="s">
-        <v>122</v>
-      </c>
-      <c r="J168" s="14"/>
+        <v>121</v>
+      </c>
+      <c r="J168" s="14" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="169" spans="9:10">
       <c r="I169" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J169" s="14"/>
     </row>
     <row r="170" spans="9:10">
       <c r="I170" t="s">
-        <v>124</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="J170" s="14"/>
     </row>
     <row r="171" spans="9:10">
       <c r="I171" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="172" spans="9:10">
       <c r="I172" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="173" spans="9:10">
+      <c r="I173" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="173" spans="9:10">
-      <c r="J173" s="8">
-        <f xml:space="preserve"> SUM(J166:J172)</f>
+    <row r="174" spans="9:10">
+      <c r="J174" s="8">
+        <f xml:space="preserve"> SUM(J167:J173)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="9:10">
+      <c r="I177" t="s">
+        <v>120</v>
+      </c>
+      <c r="J177" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="9:10">
+      <c r="I178" t="s">
+        <v>121</v>
+      </c>
+      <c r="J178" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="179" spans="9:10">
+      <c r="I179" t="s">
+        <v>122</v>
+      </c>
+      <c r="J179" s="14"/>
+    </row>
+    <row r="180" spans="9:10">
+      <c r="I180" t="s">
+        <v>123</v>
+      </c>
+      <c r="J180" s="14"/>
+    </row>
+    <row r="181" spans="9:10">
+      <c r="I181" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="182" spans="9:10">
+      <c r="I182" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="183" spans="9:10">
+      <c r="I183" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="184" spans="9:10">
+      <c r="J184" s="8">
+        <f xml:space="preserve"> SUM(J177:J183)</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J128">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="10"/>
+        <cfvo type="num" val="20"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J136">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3158,7 +3249,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J136">
+  <conditionalFormatting sqref="J148">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3180,7 +3271,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J147">
+  <conditionalFormatting sqref="J156">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3202,7 +3293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J155">
+  <conditionalFormatting sqref="J165">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3224,7 +3315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J164">
+  <conditionalFormatting sqref="J174">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3246,7 +3337,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J173">
+  <conditionalFormatting sqref="J184">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Write State of the Art
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -460,9 +460,6 @@
     <t>Images "State of the Art"</t>
   </si>
   <si>
-    <t>Write down related work "Non rigid registration"</t>
-  </si>
-  <si>
     <t>Write "general pose capture" + related paper</t>
   </si>
   <si>
@@ -494,6 +491,9 @@
   </si>
   <si>
     <t>Write State of the Art</t>
+  </si>
+  <si>
+    <t>Summarize related work "Non rigid registration"</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="G170" sqref="G170"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2840,7 +2840,7 @@
         <v>43243</v>
       </c>
       <c r="E140" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="F140">
         <v>8</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="141" spans="4:10">
       <c r="E141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F141">
         <v>8</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="142" spans="4:10">
       <c r="E142" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F142">
         <v>8</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="144" spans="4:10">
       <c r="E144" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F144">
         <v>4</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="145" spans="4:10">
       <c r="E145" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F145">
         <v>4</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="147" spans="4:10">
       <c r="E147" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F147">
         <v>6</v>
@@ -2958,7 +2958,7 @@
         <v>43252</v>
       </c>
       <c r="E150" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F150">
         <v>3</v>
@@ -2975,7 +2975,7 @@
         <v>43255</v>
       </c>
       <c r="E151" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F151">
         <v>5</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="154" spans="4:10">
       <c r="E154" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I154" t="s">
         <v>125</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="155" spans="4:10">
       <c r="E155" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I155" t="s">
         <v>126</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="156" spans="4:10">
       <c r="E156" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J156" s="8">
         <f xml:space="preserve"> SUM(J149:J155)</f>
@@ -3040,8 +3040,8 @@
       </c>
     </row>
     <row r="157" spans="4:10">
-      <c r="E157" s="48" t="s">
-        <v>156</v>
+      <c r="E157" s="26" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="4:10">

</xml_diff>

<commit_message>
Supervised methods + timetable
TODO: Unsupervised methods
Further chapters
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="162">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -481,9 +481,6 @@
     <t>Add Results + images</t>
   </si>
   <si>
-    <t>Project chapter completed + correction</t>
-  </si>
-  <si>
     <t>First thesis version + correction</t>
   </si>
   <si>
@@ -494,6 +491,21 @@
   </si>
   <si>
     <t>Summarize related work "Non rigid registration"</t>
+  </si>
+  <si>
+    <t>Write linear approach + testing!</t>
+  </si>
+  <si>
+    <t>Write feature approach</t>
+  </si>
+  <si>
+    <t>Find keyplayer</t>
+  </si>
+  <si>
+    <t>Finish project</t>
+  </si>
+  <si>
+    <t>Clean up eclipse code</t>
   </si>
 </sst>
 </file>
@@ -836,8 +848,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -986,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="95">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1031,6 +1049,9 @@
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1075,6 +1096,9 @@
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1406,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2841,7 +2865,7 @@
         <v>43243</v>
       </c>
       <c r="E140" s="54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F140" s="54">
         <v>8</v>
@@ -2854,10 +2878,10 @@
       </c>
     </row>
     <row r="141" spans="4:10">
-      <c r="E141" t="s">
+      <c r="E141" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="45">
         <v>8</v>
       </c>
       <c r="I141" t="s">
@@ -2869,7 +2893,7 @@
     </row>
     <row r="142" spans="4:10">
       <c r="E142" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F142">
         <v>8</v>
@@ -2937,9 +2961,11 @@
       </c>
     </row>
     <row r="148" spans="4:10">
+      <c r="E148" t="s">
+        <v>157</v>
+      </c>
       <c r="F148">
-        <f>SUM(F140:F147)</f>
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="J148" s="8">
         <f xml:space="preserve"> SUM(J138:J147)</f>
@@ -2947,6 +2973,12 @@
       </c>
     </row>
     <row r="149" spans="4:10">
+      <c r="E149" t="s">
+        <v>158</v>
+      </c>
+      <c r="F149">
+        <v>4</v>
+      </c>
       <c r="I149" t="s">
         <v>120</v>
       </c>
@@ -2955,14 +2987,10 @@
       </c>
     </row>
     <row r="150" spans="4:10">
-      <c r="D150" s="32">
-        <v>43252</v>
-      </c>
-      <c r="E150" t="s">
-        <v>153</v>
-      </c>
+      <c r="D150" s="32"/>
       <c r="F150">
-        <v>3</v>
+        <f>SUM(F142:F145)+SUM(F147:F149)</f>
+        <v>34</v>
       </c>
       <c r="I150" t="s">
         <v>121</v>
@@ -2972,15 +3000,6 @@
       </c>
     </row>
     <row r="151" spans="4:10">
-      <c r="D151" s="32">
-        <v>43255</v>
-      </c>
-      <c r="E151" t="s">
-        <v>154</v>
-      </c>
-      <c r="F151">
-        <v>5</v>
-      </c>
       <c r="I151" t="s">
         <v>122</v>
       </c>
@@ -2989,7 +3008,15 @@
       </c>
     </row>
     <row r="152" spans="4:10">
-      <c r="E152" s="48"/>
+      <c r="D152" s="32">
+        <v>43255</v>
+      </c>
+      <c r="E152" t="s">
+        <v>153</v>
+      </c>
+      <c r="F152">
+        <v>5</v>
+      </c>
       <c r="I152" t="s">
         <v>123</v>
       </c>
@@ -2998,10 +3025,15 @@
       </c>
     </row>
     <row r="153" spans="4:10">
-      <c r="D153" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E153" s="48"/>
+      <c r="D153" s="32">
+        <v>43259</v>
+      </c>
+      <c r="E153" t="s">
+        <v>160</v>
+      </c>
+      <c r="F153">
+        <v>8</v>
+      </c>
       <c r="I153" t="s">
         <v>124</v>
       </c>
@@ -3010,9 +3042,10 @@
       </c>
     </row>
     <row r="154" spans="4:10">
-      <c r="E154" s="48" t="s">
-        <v>149</v>
-      </c>
+      <c r="D154" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E154" s="48"/>
       <c r="I154" t="s">
         <v>125</v>
       </c>
@@ -3022,7 +3055,7 @@
     </row>
     <row r="155" spans="4:10">
       <c r="E155" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I155" t="s">
         <v>126</v>
@@ -3033,7 +3066,7 @@
     </row>
     <row r="156" spans="4:10">
       <c r="E156" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J156" s="8">
         <f xml:space="preserve"> SUM(J149:J155)</f>
@@ -3041,11 +3074,14 @@
       </c>
     </row>
     <row r="157" spans="4:10">
-      <c r="E157" s="26" t="s">
-        <v>155</v>
+      <c r="E157" s="48" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="4:10">
+      <c r="E158" s="26" t="s">
+        <v>154</v>
+      </c>
       <c r="I158" t="s">
         <v>120</v>
       </c>
@@ -3054,6 +3090,9 @@
       </c>
     </row>
     <row r="159" spans="4:10">
+      <c r="E159" s="48" t="s">
+        <v>159</v>
+      </c>
       <c r="I159" t="s">
         <v>121</v>
       </c>
@@ -3062,6 +3101,9 @@
       </c>
     </row>
     <row r="160" spans="4:10">
+      <c r="E160" s="48" t="s">
+        <v>161</v>
+      </c>
       <c r="I160" t="s">
         <v>122</v>
       </c>
@@ -3127,18 +3169,25 @@
       <c r="I169" t="s">
         <v>122</v>
       </c>
-      <c r="J169" s="14"/>
+      <c r="J169" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="170" spans="9:10">
       <c r="I170" t="s">
         <v>123</v>
       </c>
-      <c r="J170" s="14"/>
+      <c r="J170" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="171" spans="9:10">
       <c r="I171" t="s">
         <v>124</v>
       </c>
+      <c r="J171">
+        <v>8</v>
+      </c>
     </row>
     <row r="172" spans="9:10">
       <c r="I172" t="s">
@@ -3153,40 +3202,30 @@
     <row r="174" spans="9:10">
       <c r="J174" s="8">
         <f xml:space="preserve"> SUM(J167:J173)</f>
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="177" spans="9:10">
       <c r="I177" t="s">
         <v>120</v>
       </c>
-      <c r="J177" s="14">
-        <v>2</v>
-      </c>
+      <c r="J177" s="14"/>
     </row>
     <row r="178" spans="9:10">
       <c r="I178" t="s">
         <v>121</v>
       </c>
-      <c r="J178" s="14" t="s">
-        <v>86</v>
-      </c>
+      <c r="J178" s="14"/>
     </row>
     <row r="179" spans="9:10">
       <c r="I179" t="s">
         <v>122</v>
       </c>
-      <c r="J179" s="14">
-        <v>4</v>
-      </c>
     </row>
     <row r="180" spans="9:10">
       <c r="I180" t="s">
         <v>123</v>
       </c>
-      <c r="J180" s="14">
-        <v>4</v>
-      </c>
     </row>
     <row r="181" spans="9:10">
       <c r="I181" t="s">
@@ -3206,7 +3245,7 @@
     <row r="184" spans="9:10">
       <c r="J184" s="8">
         <f xml:space="preserve"> SUM(J177:J183)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of thesis
- Write final text
- Todo: Results!
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="171">
   <si>
     <t>Zeitplan Weihnachtsferien</t>
   </si>
@@ -520,13 +520,19 @@
     <t>Sa</t>
   </si>
   <si>
-    <t>Clean up code</t>
-  </si>
-  <si>
-    <t>Write &amp; Read RESULTS</t>
-  </si>
-  <si>
-    <t>Write &amp;  Read the rest</t>
+    <t>Write Linear Approach</t>
+  </si>
+  <si>
+    <t>Write Feature Approach + Conclusion</t>
+  </si>
+  <si>
+    <t>So</t>
+  </si>
+  <si>
+    <t>Create new test data</t>
+  </si>
+  <si>
+    <t>Clean up code + start scientific talk</t>
   </si>
 </sst>
 </file>
@@ -1451,16 +1457,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="5" max="6" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23">
@@ -3178,7 +3183,7 @@
         <v>163</v>
       </c>
       <c r="F166" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="167" spans="5:10">
@@ -3186,7 +3191,7 @@
         <v>164</v>
       </c>
       <c r="F167" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I167" t="s">
         <v>120</v>
@@ -3200,7 +3205,7 @@
         <v>165</v>
       </c>
       <c r="F168" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I168" t="s">
         <v>121</v>
@@ -3210,6 +3215,12 @@
       </c>
     </row>
     <row r="169" spans="5:10">
+      <c r="E169" t="s">
+        <v>168</v>
+      </c>
+      <c r="F169" t="s">
+        <v>170</v>
+      </c>
       <c r="I169" t="s">
         <v>122</v>
       </c>

</xml_diff>